<commit_message>
Made basic framework of backend server project. As a sample its user can be access, and database connection is done.
</commit_message>
<xml_diff>
--- a/documents/database/databases.xlsx
+++ b/documents/database/databases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/445c6c4e8400985e/win数据迁移/Projects/Expense Statistics App Project/documents/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{8ADEEE24-66C5-4752-B089-7156A878934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC1F06B-891D-4AE1-9B6A-6AEE1E2CB9F0}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{8ADEEE24-66C5-4752-B089-7156A878934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{703E4B94-6434-48EE-83AD-DB90F4DEEBBA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01_users" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="142">
   <si>
     <t>Table name：</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1041,8 +1041,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1193,9 +1193,7 @@
       <c r="F7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="H7" s="3"/>
       <c r="L7" s="1" t="s">
         <v>137</v>
       </c>
@@ -2822,8 +2820,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>